<commit_message>
Git diff report for release/codepush_2.0 and codepush_2.0
</commit_message>
<xml_diff>
--- a/Impacted_Files_List.xlsx
+++ b/Impacted_Files_List.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -392,9 +392,57 @@
         <v>FilePath</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>MISC</v>
+      </c>
+      <c r="B2" t="str">
+        <v>.github/workflows/testPR.yml</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>MISC</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Impacted_Files_List.xlsx</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>MISC</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Impacted_Modules_List.xlsx</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>MISC</v>
+      </c>
+      <c r="B5" t="str">
+        <v>test.txt</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>RN_LIBRARIES</v>
+      </c>
+      <c r="B6" t="str">
+        <v>package.json</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>RN_LIBRARIES</v>
+      </c>
+      <c r="B7" t="str">
+        <v>yarn.lock</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Git diff report for release/codepush_2.0 and
</commit_message>
<xml_diff>
--- a/Impacted_Files_List.xlsx
+++ b/Impacted_Files_List.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -392,57 +392,9 @@
         <v>FilePath</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>MISC</v>
-      </c>
-      <c r="B2" t="str">
-        <v>.github/workflows/testPR.yml</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>MISC</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Impacted_Files_List.xlsx</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>MISC</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Impacted_Modules_List.xlsx</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>MISC</v>
-      </c>
-      <c r="B5" t="str">
-        <v>test.txt</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>RN_LIBRARIES</v>
-      </c>
-      <c r="B6" t="str">
-        <v>package.json</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>RN_LIBRARIES</v>
-      </c>
-      <c r="B7" t="str">
-        <v>yarn.lock</v>
-      </c>
-    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>